<commit_message>
{UPDATE} capsule 002 , capsule 004, capsule 006
</commit_message>
<xml_diff>
--- a/thématique SI/006 Culture architecte SI/storyboard 006.xlsx
+++ b/thématique SI/006 Culture architecte SI/storyboard 006.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26505"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Library/Mobile Documents/com~apple~CloudDocs/Documents/pro/ISIS/2023-2024/dev/projet-FENS/thématique SI/006 Culture architecte SI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stage\projet-FENS\thématique SI\006 Culture architecte SI\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB662EC6-B0B0-A243-B1F0-4C20C0072207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3915B7B8-F983-40DB-A947-DAE58B4AFDA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2320" yWindow="120" windowWidth="35680" windowHeight="16540" xr2:uid="{A4F29CA4-E8D0-5846-A34B-CC524442BAF9}"/>
+    <workbookView xWindow="28680" yWindow="-15120" windowWidth="19440" windowHeight="15600" xr2:uid="{A4F29CA4-E8D0-5846-A34B-CC524442BAF9}"/>
   </bookViews>
   <sheets>
     <sheet name="E3-1-ISI1-4-005 et 6 SCEN" sheetId="8" r:id="rId1"/>
@@ -20,14 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -88,9 +80,9 @@
 Chaque couche isole un aspect particulier du système d'information en étant responsable des intéractions entre ses éléments.
 Chaque couche n'échangeant qu'avec ses couches adjacentes.
 Les deux premières couches forment le système informatique, l'ensemble structuré des composants matériels et logiciels et les données permettant d'automatiser tout ou partie du système métier au travers de fonctionnalités qui lui sont nécessaires.
-Enfin il est courant d'y ajouter la vue stratégie. Il s'agit de la stratégie décidée par la D.S.I. pour le S.I. en alignement avec la stratégie de l'organisation.
 Le système métier est formé des services et processus de l'entreprise, des organisations qui les mettent en œuvre et des objets métier associés.
-Un objet métier est un concept ou une abstraction ayant un sens pour des acteurs (partie prenante interne) d'une organisation (par exemple une entreprise). L'objet métier permet de décrire les entités manipulées par les acteurs dans le cadre de la description du métier.</t>
+Un objet métier est un concept ou une abstraction ayant un sens pour des acteurs (partie prenante interne) d'une organisation (par exemple une entreprise). L'objet métier permet de décrire les entités manipulées par les acteurs dans le cadre de la description du métier.
+Enfin il est courant d'y ajouter la vue stratégie. Il s'agit de la stratégie décidée par la D.S.I. pour le S.I. en alignement avec la stratégie de l'organisation.</t>
   </si>
 </sst>
 </file>
@@ -621,20 +613,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2AF475-8297-9B48-A5BF-C8EFBB80C1A0}">
   <dimension ref="A1:E9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="143" zoomScaleNormal="143" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
-    <col min="2" max="2" width="16.83203125" customWidth="1"/>
-    <col min="3" max="3" width="58.1640625" customWidth="1"/>
-    <col min="4" max="4" width="53.33203125" style="5" customWidth="1"/>
-    <col min="5" max="6" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="17.796875" customWidth="1"/>
+    <col min="2" max="2" width="16.796875" customWidth="1"/>
+    <col min="3" max="3" width="58.19921875" customWidth="1"/>
+    <col min="4" max="4" width="53.296875" style="5" customWidth="1"/>
+    <col min="5" max="6" width="26.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>9</v>
       </c>
@@ -642,7 +634,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A2" s="4" t="s">
         <v>10</v>
       </c>
@@ -650,23 +642,23 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
       <c r="B4" s="3"/>
     </row>
-    <row r="6" spans="1:5" ht="154" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" ht="154.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>11</v>
       </c>
@@ -683,7 +675,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="254" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" ht="253.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="1" t="s">
         <v>12</v>
       </c>
@@ -691,7 +683,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="236" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" ht="235.95" customHeight="1" x14ac:dyDescent="0.3">
       <c r="D9" s="7" t="s">
         <v>13</v>
       </c>

</xml_diff>